<commit_message>
worked on some exceptions
</commit_message>
<xml_diff>
--- a/Project/excel_source/major_abbreviations.xlsx
+++ b/Project/excel_source/major_abbreviations.xlsx
@@ -696,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>